<commit_message>
_ MaJ EnergyAlternativesPlaning  * possibilité d'utiliser la fléxibilité en noeud simple _ Création de ES_Electric_System_Subects  * Codes et notebooks pour noeuds simple, douple noeuds et 7 noeuds
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/parameters_planification.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/parameters_planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F112C5-AC2B-4459-967B-8B27556FA0E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D24DD74-8405-4AD4-8F6D-1B8E820CBF36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="492" windowWidth="23748" windowHeight="11760" activeTab="1" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
+    <workbookView xWindow="5055" yWindow="495" windowWidth="23745" windowHeight="11760" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
   </bookViews>
   <sheets>
     <sheet name="TECHNOLOGIES" sheetId="5" r:id="rId1"/>
@@ -697,18 +697,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548A25F0-7C8F-4D52-A757-E2D4BFA810AD}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.09765625" customWidth="1"/>
-    <col min="3" max="7" width="11.19921875" style="6"/>
-    <col min="13" max="13" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="7" width="11.25" style="6"/>
+    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
@@ -743,7 +743,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -817,7 +817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -854,7 +854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -881,7 +881,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
@@ -908,7 +908,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -927,7 +927,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -946,7 +946,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -965,7 +965,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -992,7 +992,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>640.35140000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>3</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>40</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>4</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>16</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>17</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>18</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>1</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>2</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>3</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>40</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>46</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>4</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>15</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>16</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>17</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>18</v>
       </c>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>26</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>1</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>2</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>3</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>40</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>46</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>15</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>16</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>17</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>18</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>26</v>
       </c>
@@ -2204,21 +2204,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.09765625" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.09765625" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" style="6"/>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="11.25" style="6"/>
     <col min="5" max="7" width="19.5" style="6" customWidth="1"/>
     <col min="8" max="8" width="18.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2440,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -2549,7 +2549,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
@@ -2705,7 +2705,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -2735,7 +2735,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>26</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>0</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2828,7 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>2</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -2870,7 +2870,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -2888,7 +2888,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>3</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>40</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
@@ -2962,7 +2962,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>46</v>
       </c>
@@ -2980,7 +2980,7 @@
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>15</v>
       </c>
@@ -3010,7 +3010,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>16</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>17</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>18</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>26</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>1</v>
       </c>
@@ -3107,7 +3107,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>2</v>
       </c>
@@ -3125,7 +3125,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>2</v>
       </c>
@@ -3143,7 +3143,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>2</v>
       </c>
@@ -3161,7 +3161,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>3</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>40</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>40</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>46</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
         <v>46</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>4</v>
       </c>
@@ -3261,7 +3261,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
         <v>15</v>
       </c>
@@ -3275,7 +3275,7 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="s">
         <v>16</v>
       </c>
@@ -3291,7 +3291,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
         <v>17</v>
       </c>
@@ -3307,7 +3307,7 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
         <v>18</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>26</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>1</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
         <v>2</v>
       </c>
@@ -3386,7 +3386,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
         <v>2</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>2</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>3</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>40</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>40</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>46</v>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>46</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>4</v>
       </c>
@@ -3522,7 +3522,7 @@
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>15</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>16</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
         <v>17</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
         <v>18</v>
       </c>
@@ -3582,7 +3582,7 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>26</v>
       </c>
@@ -3608,13 +3608,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7586E3A9-C0EE-6F42-8EFF-5D7691C2A1FF}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>35</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3672,8 +3672,7 @@
         <v>2015</v>
       </c>
       <c r="C3" s="10">
-        <f>0.000001*5*16900</f>
-        <v>8.4499999999999992E-2</v>
+        <v>-3</v>
       </c>
       <c r="D3" s="4">
         <f>400*(-0.5/($B$50-$B$2)*B3+(1+0.5/($B$50-$B$2)*$B$2))</f>
@@ -3688,7 +3687,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3712,7 +3711,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3734,7 +3733,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -3756,7 +3755,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3778,7 +3777,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3800,7 +3799,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -3822,7 +3821,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -3844,7 +3843,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3866,7 +3865,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
@@ -3888,7 +3887,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>22</v>
       </c>
@@ -3910,7 +3909,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -3934,7 +3933,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -3942,8 +3941,7 @@
         <v>2027</v>
       </c>
       <c r="C15" s="10">
-        <f>0.000001*5*16900</f>
-        <v>8.4499999999999992E-2</v>
+        <v>-3</v>
       </c>
       <c r="D15" s="4">
         <f>400*(-0.5/($B$50-$B$2)*B15+(1+0.5/($B$50-$B$2)*$B$2))</f>
@@ -3958,7 +3956,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -3982,7 +3980,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -4004,7 +4002,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -4026,7 +4024,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -4048,7 +4046,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -4071,7 +4069,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -4094,7 +4092,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -4116,7 +4114,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -4138,7 +4136,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
@@ -4161,7 +4159,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
@@ -4184,7 +4182,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
@@ -4208,7 +4206,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>11</v>
       </c>
@@ -4216,8 +4214,7 @@
         <v>2030</v>
       </c>
       <c r="C27" s="10">
-        <f>0.000001*5*16900</f>
-        <v>8.4499999999999992E-2</v>
+        <v>-3</v>
       </c>
       <c r="D27" s="4">
         <f>400*(-0.5/($B$50-$B$2)*B27+(1+0.5/($B$50-$B$2)*$B$2))</f>
@@ -4232,7 +4229,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
@@ -4256,7 +4253,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
@@ -4264,7 +4261,7 @@
         <v>2030</v>
       </c>
       <c r="C29" s="10">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4">
         <v>60</v>
@@ -4278,7 +4275,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>14</v>
       </c>
@@ -4300,7 +4297,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
@@ -4322,7 +4319,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
@@ -4344,7 +4341,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>24</v>
       </c>
@@ -4366,7 +4363,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
@@ -4388,7 +4385,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>20</v>
       </c>
@@ -4410,7 +4407,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>21</v>
       </c>
@@ -4433,7 +4430,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>22</v>
       </c>
@@ -4456,7 +4453,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>10</v>
       </c>
@@ -4478,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>11</v>
       </c>
@@ -4486,8 +4483,7 @@
         <v>2040</v>
       </c>
       <c r="C39" s="10">
-        <f>0.000001*5*16900</f>
-        <v>8.4499999999999992E-2</v>
+        <v>-3</v>
       </c>
       <c r="D39" s="4">
         <f>400*(-0.5/($B$50-$B$2)*B39+(1+0.5/($B$50-$B$2)*$B$2))</f>
@@ -4500,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>12</v>
       </c>
@@ -4522,7 +4518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>13</v>
       </c>
@@ -4530,7 +4526,7 @@
         <v>2040</v>
       </c>
       <c r="C41" s="10">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="D41" s="4">
         <v>60</v>
@@ -4542,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>14</v>
       </c>
@@ -4562,7 +4558,7 @@
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>6</v>
       </c>
@@ -4582,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>23</v>
       </c>
@@ -4603,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>24</v>
       </c>
@@ -4624,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
@@ -4644,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>20</v>
       </c>
@@ -4664,7 +4660,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>21</v>
       </c>
@@ -4685,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>22</v>
       </c>
@@ -4706,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>10</v>
       </c>
@@ -4728,7 +4724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>11</v>
       </c>
@@ -4736,8 +4732,7 @@
         <v>2050</v>
       </c>
       <c r="C51" s="10">
-        <f>0.000001*5*16900</f>
-        <v>8.4499999999999992E-2</v>
+        <v>-3</v>
       </c>
       <c r="D51" s="4">
         <f>400*(-0.5/($B$50-$B$2)*B51+(1+0.5/($B$50-$B$2)*$B$2))</f>
@@ -4750,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>12</v>
       </c>
@@ -4772,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>13</v>
       </c>
@@ -4780,7 +4775,7 @@
         <v>2050</v>
       </c>
       <c r="C53" s="10">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="D53" s="4">
         <v>60</v>
@@ -4792,7 +4787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>14</v>
       </c>
@@ -4812,7 +4807,7 @@
       </c>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>6</v>
       </c>
@@ -4832,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>23</v>
       </c>
@@ -4853,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>24</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>19</v>
       </c>
@@ -4894,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>20</v>
       </c>
@@ -4914,7 +4909,7 @@
         <v>17000000</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>21</v>
       </c>
@@ -4935,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
         <v>22</v>
       </c>
@@ -4965,17 +4960,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CECC86B-EA41-AD43-AFC8-B7990C2DC2F5}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="14.8984375" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="11.19921875" style="7"/>
+    <col min="1" max="3" width="14.875" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="11.25" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
@@ -5022,7 +5017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -5046,7 +5041,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
@@ -5074,7 +5069,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
@@ -5102,7 +5097,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -5130,7 +5125,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -5156,7 +5151,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>26</v>
       </c>
@@ -5180,7 +5175,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -5209,7 +5204,7 @@
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -5237,7 +5232,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -5271,7 +5266,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -5307,7 +5302,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -5343,7 +5338,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -5373,7 +5368,7 @@
       </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -5407,7 +5402,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -5439,7 +5434,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -5473,7 +5468,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -5507,7 +5502,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>4</v>
       </c>
@@ -5531,7 +5526,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -5558,7 +5553,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>16</v>
       </c>
@@ -5585,7 +5580,7 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
@@ -5612,7 +5607,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>18</v>
       </c>
@@ -5637,7 +5632,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>26</v>
       </c>
@@ -5660,7 +5655,7 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
@@ -5688,7 +5683,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -5715,7 +5710,7 @@
       </c>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -5748,7 +5743,7 @@
       </c>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -5783,7 +5778,7 @@
       </c>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -5818,7 +5813,7 @@
       </c>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -5847,7 +5842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
@@ -5880,7 +5875,7 @@
       </c>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
@@ -5911,7 +5906,7 @@
       </c>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
@@ -5944,7 +5939,7 @@
       </c>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -5977,7 +5972,7 @@
       </c>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>4</v>
       </c>
@@ -6000,7 +5995,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>15</v>
       </c>
@@ -6027,7 +6022,7 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>16</v>
       </c>
@@ -6054,7 +6049,7 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>17</v>
       </c>
@@ -6081,7 +6076,7 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>18</v>
       </c>
@@ -6106,7 +6101,7 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>26</v>
       </c>
@@ -6129,7 +6124,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>0</v>
       </c>
@@ -6157,7 +6152,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
@@ -6184,7 +6179,7 @@
       </c>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -6217,7 +6212,7 @@
       </c>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>2</v>
       </c>
@@ -6252,7 +6247,7 @@
       </c>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -6287,7 +6282,7 @@
       </c>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
@@ -6316,7 +6311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>40</v>
       </c>
@@ -6349,7 +6344,7 @@
       </c>
       <c r="O46" s="4"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>40</v>
       </c>
@@ -6380,7 +6375,7 @@
       </c>
       <c r="O47" s="4"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
@@ -6413,7 +6408,7 @@
       </c>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
@@ -6446,7 +6441,7 @@
       </c>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
         <v>4</v>
       </c>
@@ -6469,7 +6464,7 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>15</v>
       </c>
@@ -6496,7 +6491,7 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>16</v>
       </c>
@@ -6523,7 +6518,7 @@
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
         <v>17</v>
       </c>
@@ -6550,7 +6545,7 @@
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>18</v>
       </c>
@@ -6575,7 +6570,7 @@
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>26</v>
       </c>
@@ -6598,7 +6593,7 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>0</v>
       </c>
@@ -6626,7 +6621,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>1</v>
       </c>
@@ -6653,7 +6648,7 @@
       </c>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>2</v>
       </c>
@@ -6686,7 +6681,7 @@
       </c>
       <c r="O58" s="4"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
         <v>2</v>
       </c>
@@ -6721,7 +6716,7 @@
       </c>
       <c r="O59" s="4"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>2</v>
       </c>
@@ -6756,7 +6751,7 @@
       </c>
       <c r="O60" s="4"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
         <v>3</v>
       </c>
@@ -6785,7 +6780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="s">
         <v>40</v>
       </c>
@@ -6818,7 +6813,7 @@
       </c>
       <c r="O62" s="4"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
         <v>40</v>
       </c>
@@ -6849,7 +6844,7 @@
       </c>
       <c r="O63" s="4"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
         <v>46</v>
       </c>
@@ -6882,7 +6877,7 @@
       </c>
       <c r="O64" s="4"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>46</v>
       </c>
@@ -6915,7 +6910,7 @@
       </c>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>4</v>
       </c>
@@ -6938,7 +6933,7 @@
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>15</v>
       </c>
@@ -6965,7 +6960,7 @@
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>16</v>
       </c>
@@ -6992,7 +6987,7 @@
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>17</v>
       </c>
@@ -7019,7 +7014,7 @@
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>18</v>
       </c>
@@ -7044,7 +7039,7 @@
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>26</v>
       </c>
@@ -7067,7 +7062,7 @@
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>0</v>
       </c>
@@ -7095,7 +7090,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>1</v>
       </c>
@@ -7122,7 +7117,7 @@
       </c>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>2</v>
       </c>
@@ -7155,7 +7150,7 @@
       </c>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>2</v>
       </c>
@@ -7190,7 +7185,7 @@
       </c>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>2</v>
       </c>
@@ -7225,7 +7220,7 @@
       </c>
       <c r="O76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>3</v>
       </c>
@@ -7254,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>40</v>
       </c>
@@ -7287,7 +7282,7 @@
       </c>
       <c r="O78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
         <v>40</v>
       </c>
@@ -7318,7 +7313,7 @@
       </c>
       <c r="O79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
         <v>46</v>
       </c>
@@ -7351,7 +7346,7 @@
       </c>
       <c r="O80" s="4"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>46</v>
       </c>

</xml_diff>